<commit_message>
Contact page worked up, Calendar page started
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/CogmentoTestData.xlsx
+++ b/src/main/resources/testData/CogmentoTestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkati\Downloads\Katia-cogmento-crm-automatiaon\src\main\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9325E9-2E29-41C2-95E8-18FE6EABF713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7642843-F3A4-489D-A2BE-752514CF9D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1470" windowWidth="21600" windowHeight="11970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="calls" sheetId="2" r:id="rId2"/>
-    <sheet name="calendar" sheetId="3" r:id="rId3"/>
+    <sheet name="calendar" sheetId="6" r:id="rId3"/>
     <sheet name="deals" sheetId="5" r:id="rId4"/>
     <sheet name="documents" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>firstname</t>
   </si>
@@ -243,6 +243,42 @@
   </si>
   <si>
     <t>confirmDeletion</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>Bosco Place</t>
+  </si>
+  <si>
+    <t>re union</t>
+  </si>
+  <si>
+    <t>Ferndale, Michigan</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>addNote</t>
+  </si>
+  <si>
+    <t>Remember Me</t>
   </si>
 </sst>
 </file>
@@ -868,24 +904,68 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A442C6F6-62B3-405F-B3D9-88E0DCABA9D0}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2">
-        <v>44957</v>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -893,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C79A4EB-347D-4107-9046-127E08006059}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>